<commit_message>
diagrama clases y gantt actualizados
</commit_message>
<xml_diff>
--- a/Calendarizacion/Diagrama Gantt.xlsx
+++ b/Calendarizacion/Diagrama Gantt.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Actividades:</t>
   </si>
@@ -48,19 +48,34 @@
     <t>Mockups</t>
   </si>
   <si>
-    <t>Diagramas : casos de uso/ Especificacion/Estado</t>
-  </si>
-  <si>
-    <t>Base de datos (ABM)</t>
-  </si>
-  <si>
-    <t>Desarrollo aplicación</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Inicio Proyecto</t>
-  </si>
-  <si>
-    <t>Fin Proyecto</t>
+    <t xml:space="preserve">Base de datos  </t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Notificaciones</t>
+  </si>
+  <si>
+    <t>Diccionario de datos</t>
+  </si>
+  <si>
+    <t>Reportes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Casos de uso/ Especificacion/ Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funciones ABM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otras funcionalidades </t>
+  </si>
+  <si>
+    <t>Interfaz grafica</t>
   </si>
 </sst>
 </file>
@@ -193,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -217,6 +232,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -308,9 +326,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$D$2:$D$9</c:f>
+              <c:f>Hoja1!$D$2:$D$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Relevamiento</c:v>
                 </c:pt>
@@ -327,23 +345,26 @@
                   <c:v>Mockups</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Diagramas : casos de uso/ Especificacion/Estado</c:v>
+                  <c:v> Casos de uso/ Especificacion/ Estado</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Base de datos (ABM)</c:v>
+                  <c:v>Base de datos  </c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Desarrollo aplicación</c:v>
+                  <c:v>Funciones ABM </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Roles</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$E$2:$E$9</c:f>
+              <c:f>Hoja1!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>43684</c:v>
                 </c:pt>
@@ -366,6 +387,9 @@
                   <c:v>43726</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>43733</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>43769</c:v>
                 </c:pt>
               </c:numCache>
@@ -392,9 +416,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$D$2:$D$9</c:f>
+              <c:f>Hoja1!$D$2:$D$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Relevamiento</c:v>
                 </c:pt>
@@ -411,23 +435,26 @@
                   <c:v>Mockups</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Diagramas : casos de uso/ Especificacion/Estado</c:v>
+                  <c:v> Casos de uso/ Especificacion/ Estado</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Base de datos (ABM)</c:v>
+                  <c:v>Base de datos  </c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Desarrollo aplicación</c:v>
+                  <c:v>Funciones ABM </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Roles</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$F$2:$F$9</c:f>
+              <c:f>Hoja1!$F$2:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>14</c:v>
                 </c:pt>
@@ -450,7 +477,10 @@
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>152</c:v>
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -471,11 +501,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="181906432"/>
-        <c:axId val="181916416"/>
+        <c:axId val="193113088"/>
+        <c:axId val="193123072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181906432"/>
+        <c:axId val="193113088"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -529,7 +559,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181916416"/>
+        <c:crossAx val="193123072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -537,7 +567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181916416"/>
+        <c:axId val="193123072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="43684"/>
@@ -602,7 +632,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181906432"/>
+        <c:crossAx val="193113088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -621,7 +651,7 @@
   <c:spPr>
     <a:blipFill dpi="0" rotWithShape="1">
       <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-        <a:alphaModFix amt="62000"/>
+        <a:alphaModFix amt="31000"/>
       </a:blip>
       <a:srcRect/>
       <a:stretch>
@@ -657,565 +687,20 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1492,7 +977,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1500,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,7 +1039,7 @@
         <v>43698</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F9" si="0">G3-E3</f>
+        <f t="shared" ref="F3:F8" si="0">G3-E3</f>
         <v>14</v>
       </c>
       <c r="G3" s="3">
@@ -1563,13 +1048,8 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="8">
-        <f>E2</f>
-        <v>43684</v>
-      </c>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1586,13 +1066,8 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="10">
-        <f>G9</f>
-        <v>43921</v>
-      </c>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1624,7 +1099,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E7" s="3">
         <v>43719</v>
@@ -1639,7 +1114,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3">
         <v>43726</v>
@@ -1654,16 +1129,121 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3">
+        <v>43733</v>
+      </c>
+      <c r="F9" s="1">
+        <f>G9-E9</f>
+        <v>43</v>
+      </c>
+      <c r="G9" s="3">
+        <v>43776</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3">
+        <v>43769</v>
+      </c>
+      <c r="F10" s="1">
+        <f>G10-E10</f>
+        <v>21</v>
+      </c>
+      <c r="G10" s="3">
+        <v>43790</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3">
-        <v>43769</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>152</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="E11" s="3">
+        <v>43790</v>
+      </c>
+      <c r="F11" s="1">
+        <f>G11-E11</f>
+        <v>14</v>
+      </c>
+      <c r="G11" s="3">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3">
+        <v>43726</v>
+      </c>
+      <c r="F12" s="1">
+        <f>G12-E12</f>
+        <v>78</v>
+      </c>
+      <c r="G12" s="3">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3">
+        <v>43804</v>
+      </c>
+      <c r="F13" s="1">
+        <f>G13-E13</f>
+        <v>87</v>
+      </c>
+      <c r="G13" s="3">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="3">
+        <v>43790</v>
+      </c>
+      <c r="F14" s="11">
+        <f>G14-E14</f>
+        <v>131</v>
+      </c>
+      <c r="G14" s="3">
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="3">
+        <v>43891</v>
+      </c>
+      <c r="F15" s="1">
+        <f>G15-E15</f>
+        <v>30</v>
+      </c>
+      <c r="G15" s="3">
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="3">
+        <v>43891</v>
+      </c>
+      <c r="F16" s="1">
+        <f>G16-E16</f>
+        <v>30</v>
+      </c>
+      <c r="G16" s="3">
         <v>43921</v>
       </c>
     </row>

</xml_diff>